<commit_message>
motor analitico semi finalizado
</commit_message>
<xml_diff>
--- a/test/Asistencia Alfabetizacion Digital.xlsx
+++ b/test/Asistencia Alfabetizacion Digital.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Personal Sebastian\universidad\Desarrollo De Proyecto Tecnologico\Desarrollo_Proyc_Tecn\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3926FD-F4A2-44D4-919D-FE775AD407EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950FC221-7808-4DEA-A661-D42A42DCC981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22920" yWindow="660" windowWidth="21600" windowHeight="11295" xr2:uid="{D921C168-2EC5-442A-B4B7-C9A9E86E61A2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D921C168-2EC5-442A-B4B7-C9A9E86E61A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="112">
   <si>
     <t>N°</t>
   </si>
@@ -207,9 +207,6 @@
   </si>
   <si>
     <t>belindaluna9874@gmail.com</t>
-  </si>
-  <si>
-    <t>Manuel Estraño</t>
   </si>
   <si>
     <t>K</t>
@@ -381,7 +378,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,6 +424,14 @@
       <sz val="10"/>
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -533,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -611,6 +616,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -946,15 +952,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B30B195-F3B4-47DE-9066-B8BE785E8361}">
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:S38"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1019,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1072,7 +1078,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1131,7 +1137,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="39" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1190,7 +1196,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1249,7 +1255,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1308,7 +1314,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1367,7 +1373,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1424,7 +1430,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1541,8 +1547,9 @@
       <c r="S10" s="16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="U10" s="29"/>
+    </row>
+    <row r="11" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1601,7 +1608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="39" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1656,29 +1663,43 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="39" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="13"/>
+      <c r="C13" s="10">
+        <v>27000489</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="E13" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F13" s="13">
-        <v>931353305</v>
-      </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="16"/>
+        <v>949974400</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="11">
+        <v>69</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="K13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="16"/>
+      <c r="L13" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="M13" s="16" t="s">
         <v>26</v>
       </c>
@@ -1701,42 +1722,42 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="10">
-        <v>27000489</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>58</v>
+        <v>4160900</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" s="13">
-        <v>949974400</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>60</v>
+        <v>967489586</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="H14" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="11">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="K14" s="15" t="s">
         <v>24</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="M14" s="16" t="s">
         <v>26</v>
@@ -1760,33 +1781,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="39" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="10">
-        <v>4160900</v>
+        <v>10020839</v>
       </c>
       <c r="D15" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F15" s="13">
-        <v>967489586</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>62</v>
+        <v>945572714</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="11">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="J15" s="15" t="s">
         <v>23</v>
@@ -1795,7 +1816,7 @@
         <v>24</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="M15" s="16" t="s">
         <v>26</v>
@@ -1819,33 +1840,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="39" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="10">
-        <v>10020839</v>
+        <v>6875320</v>
       </c>
       <c r="D16" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F16" s="13">
-        <v>945572714</v>
+        <v>982394563</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H16" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="11">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="J16" s="15" t="s">
         <v>23</v>
@@ -1854,7 +1875,7 @@
         <v>24</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M16" s="16" t="s">
         <v>26</v>
@@ -1878,33 +1899,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="10">
-        <v>6875320</v>
+      <c r="C17" s="22">
+        <v>6364137</v>
       </c>
       <c r="D17" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F17" s="13">
-        <v>982394563</v>
+        <v>9892836649</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I17" s="11">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J17" s="15" t="s">
         <v>23</v>
@@ -1913,7 +1934,7 @@
         <v>24</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="M17" s="16" t="s">
         <v>26</v>
@@ -1937,33 +1958,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="22">
-        <v>6364137</v>
+      <c r="C18" s="18">
+        <v>5394449</v>
       </c>
       <c r="D18" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F18" s="13">
-        <v>9892836649</v>
+        <v>974512586</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="11">
-        <v>64</v>
+        <v>70</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="8">
+        <v>75</v>
       </c>
       <c r="J18" s="15" t="s">
         <v>23</v>
@@ -1971,8 +1992,8 @@
       <c r="K18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="15" t="s">
-        <v>69</v>
+      <c r="L18" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="M18" s="16" t="s">
         <v>26</v>
@@ -1998,40 +2019,40 @@
     </row>
     <row r="19" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="18">
-        <v>5394449</v>
+        <v>7643511</v>
       </c>
       <c r="D19" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F19" s="13">
-        <v>974512586</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>71</v>
+        <v>997992842</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="H19" s="16" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="8">
-        <v>75</v>
-      </c>
-      <c r="J19" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" s="16" t="s">
         <v>23</v>
       </c>
       <c r="K19" s="15" t="s">
         <v>24</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M19" s="16" t="s">
         <v>26</v>
@@ -2057,40 +2078,40 @@
     </row>
     <row r="20" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="18">
-        <v>7643511</v>
+      <c r="C20" s="10">
+        <v>6006331</v>
       </c>
       <c r="D20" s="13">
         <v>1</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F20" s="13">
-        <v>997992842</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>74</v>
+        <v>987977033</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>75</v>
       </c>
       <c r="H20" s="16" t="s">
         <v>33</v>
       </c>
       <c r="I20" s="8">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J20" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="16" t="s">
         <v>24</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="M20" s="16" t="s">
         <v>26</v>
@@ -2116,40 +2137,40 @@
     </row>
     <row r="21" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="10">
-        <v>6006331</v>
+        <v>5428349</v>
       </c>
       <c r="D21" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F21" s="13">
-        <v>987977033</v>
+        <v>926118920</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" s="8">
-        <v>74</v>
-      </c>
-      <c r="J21" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="11">
+        <v>79</v>
+      </c>
+      <c r="J21" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21" s="16" t="s">
-        <v>77</v>
+      <c r="K21" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="M21" s="16" t="s">
         <v>26</v>
@@ -2175,31 +2196,31 @@
     </row>
     <row r="22" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="10">
-        <v>5428349</v>
+        <v>13039458</v>
       </c>
       <c r="D22" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F22" s="13">
-        <v>926118920</v>
+        <v>952550701</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="I22" s="11">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="J22" s="15" t="s">
         <v>23</v>
@@ -2208,7 +2229,7 @@
         <v>24</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="M22" s="16" t="s">
         <v>26</v>
@@ -2234,31 +2255,31 @@
     </row>
     <row r="23" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="10">
-        <v>13039458</v>
+        <v>6559814</v>
       </c>
       <c r="D23" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F23" s="13">
-        <v>952550701</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>82</v>
+        <v>996914073</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="H23" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I23" s="11">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="J23" s="15" t="s">
         <v>23</v>
@@ -2267,7 +2288,7 @@
         <v>24</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="M23" s="16" t="s">
         <v>26</v>
@@ -2293,31 +2314,31 @@
     </row>
     <row r="24" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="10">
-        <v>6559814</v>
+        <v>7009839</v>
       </c>
       <c r="D24" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E24" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="13">
+        <v>946473923</v>
+      </c>
+      <c r="G24" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="F24" s="13">
-        <v>996914073</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>84</v>
       </c>
       <c r="H24" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I24" s="11">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="J24" s="15" t="s">
         <v>23</v>
@@ -2326,7 +2347,7 @@
         <v>24</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M24" s="16" t="s">
         <v>26</v>
@@ -2350,33 +2371,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="10">
-        <v>7009839</v>
+      <c r="C25" s="24">
+        <v>6079201</v>
       </c>
       <c r="D25" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>85</v>
       </c>
       <c r="F25" s="13">
-        <v>946473923</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>84</v>
+        <v>926189209</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I25" s="11">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="J25" s="15" t="s">
         <v>23</v>
@@ -2385,7 +2406,7 @@
         <v>24</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="M25" s="16" t="s">
         <v>26</v>
@@ -2409,42 +2430,42 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="24">
-        <v>6079201</v>
+        <v>93651766</v>
       </c>
       <c r="D26" s="13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F26" s="13">
-        <v>926189209</v>
+        <v>992093253</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I26" s="11">
-        <v>81</v>
-      </c>
-      <c r="J26" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="8">
+        <v>62</v>
+      </c>
+      <c r="J26" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K26" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L26" s="15" t="s">
-        <v>80</v>
+      <c r="K26" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="M26" s="16" t="s">
         <v>26</v>
@@ -2470,40 +2491,40 @@
     </row>
     <row r="27" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="24">
-        <v>93651766</v>
+      <c r="C27" s="10">
+        <v>26769185</v>
       </c>
       <c r="D27" s="13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F27" s="13">
-        <v>992093253</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="8">
-        <v>62</v>
-      </c>
-      <c r="J27" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>43</v>
+        <v>976074731</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="11">
+        <v>58</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="M27" s="16" t="s">
         <v>26</v>
@@ -2527,36 +2548,36 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="10">
-        <v>26769185</v>
-      </c>
-      <c r="D28" s="13">
-        <v>1</v>
+        <v>5785555</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F28" s="13">
-        <v>976074731</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>91</v>
+        <v>990898897</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>92</v>
       </c>
       <c r="H28" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I28" s="11">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="K28" s="15" t="s">
         <v>24</v>
@@ -2586,33 +2607,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="10">
-        <v>5785555</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>58</v>
+        <v>6764257</v>
+      </c>
+      <c r="D29" s="13">
+        <v>0</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F29" s="13">
-        <v>990898897</v>
+        <v>942948861</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H29" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I29" s="11">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J29" s="15" t="s">
         <v>23</v>
@@ -2621,7 +2642,7 @@
         <v>24</v>
       </c>
       <c r="L29" s="15" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="M29" s="16" t="s">
         <v>26</v>
@@ -2647,31 +2668,31 @@
     </row>
     <row r="30" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="10">
-        <v>6764257</v>
+        <v>7105406</v>
       </c>
       <c r="D30" s="13">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F30" s="13">
-        <v>942948861</v>
+        <v>982001309</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I30" s="11">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J30" s="15" t="s">
         <v>23</v>
@@ -2680,7 +2701,7 @@
         <v>24</v>
       </c>
       <c r="L30" s="15" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="M30" s="16" t="s">
         <v>26</v>
@@ -2704,27 +2725,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="10">
-        <v>7105406</v>
+      <c r="C31" s="18">
+        <v>7627781</v>
       </c>
       <c r="D31" s="13">
         <v>8</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>96</v>
+      <c r="E31" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="F31" s="13">
-        <v>982001309</v>
+        <v>946180239</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H31" s="15" t="s">
         <v>22</v>
@@ -2739,7 +2760,7 @@
         <v>24</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="M31" s="16" t="s">
         <v>26</v>
@@ -2763,33 +2784,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="18">
-        <v>7627781</v>
+      <c r="C32" s="10">
+        <v>7621664</v>
       </c>
       <c r="D32" s="13">
-        <v>8</v>
-      </c>
-      <c r="E32" s="27" t="s">
-        <v>99</v>
+        <v>9</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="F32" s="13">
-        <v>946180239</v>
+        <v>975048401</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="I32" s="11">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="J32" s="15" t="s">
         <v>23</v>
@@ -2798,7 +2819,7 @@
         <v>24</v>
       </c>
       <c r="L32" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M32" s="16" t="s">
         <v>26</v>
@@ -2824,31 +2845,31 @@
     </row>
     <row r="33" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="10">
-        <v>7621664</v>
+        <v>7378766</v>
       </c>
       <c r="D33" s="13">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F33" s="13">
-        <v>975048401</v>
+        <v>993093481</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H33" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I33" s="11">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J33" s="15" t="s">
         <v>23</v>
@@ -2857,7 +2878,7 @@
         <v>24</v>
       </c>
       <c r="L33" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="M33" s="16" t="s">
         <v>26</v>
@@ -2883,31 +2904,31 @@
     </row>
     <row r="34" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="10">
-        <v>7378766</v>
+        <v>9880869</v>
       </c>
       <c r="D34" s="13">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F34" s="13">
-        <v>993093481</v>
+        <v>950798878</v>
       </c>
       <c r="G34" s="21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H34" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I34" s="11">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J34" s="15" t="s">
         <v>23</v>
@@ -2916,7 +2937,7 @@
         <v>24</v>
       </c>
       <c r="L34" s="15" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="M34" s="16" t="s">
         <v>26</v>
@@ -2942,31 +2963,31 @@
     </row>
     <row r="35" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="10">
-        <v>9880869</v>
+      <c r="C35" s="18">
+        <v>7488759</v>
       </c>
       <c r="D35" s="13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F35" s="13">
-        <v>950798878</v>
+        <v>962086672</v>
       </c>
       <c r="G35" s="21" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H35" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="I35" s="11">
-        <v>56</v>
+      <c r="I35" s="8">
+        <v>70</v>
       </c>
       <c r="J35" s="15" t="s">
         <v>23</v>
@@ -2974,8 +2995,8 @@
       <c r="K35" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L35" s="15" t="s">
-        <v>107</v>
+      <c r="L35" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="M35" s="16" t="s">
         <v>26</v>
@@ -3001,31 +3022,31 @@
     </row>
     <row r="36" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="18">
-        <v>7488759</v>
-      </c>
-      <c r="D36" s="13">
-        <v>7</v>
+      <c r="C36" s="10">
+        <v>6344507</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F36" s="13">
-        <v>962086672</v>
-      </c>
-      <c r="G36" s="21" t="s">
-        <v>109</v>
+        <v>973392924</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="H36" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="I36" s="8">
-        <v>70</v>
+      <c r="I36" s="11">
+        <v>74</v>
       </c>
       <c r="J36" s="15" t="s">
         <v>23</v>
@@ -3033,8 +3054,8 @@
       <c r="K36" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L36" s="16" t="s">
-        <v>34</v>
+      <c r="L36" s="15" t="s">
+        <v>110</v>
       </c>
       <c r="M36" s="16" t="s">
         <v>26</v>
@@ -3060,41 +3081,25 @@
     </row>
     <row r="37" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="10">
-        <v>6344507</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>58</v>
-      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="13"/>
       <c r="E37" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="F37" s="13">
-        <v>973392924</v>
-      </c>
-      <c r="G37" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I37" s="11">
-        <v>74</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>23</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="F37" s="28"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="16"/>
       <c r="K37" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L37" s="15" t="s">
-        <v>111</v>
-      </c>
+      <c r="L37" s="16"/>
       <c r="M37" s="16" t="s">
         <v>26</v>
       </c>
@@ -3114,58 +3119,15 @@
         <v>29</v>
       </c>
       <c r="S37" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="39" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
-        <v>37</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="F38" s="28"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L38" s="16"/>
-      <c r="M38" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N38" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="O38" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="P38" s="17">
-        <v>45299</v>
-      </c>
-      <c r="Q38" s="17">
-        <v>45303</v>
-      </c>
-      <c r="R38" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="S38" s="16" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G10" r:id="rId1" xr:uid="{2DA1698F-A361-4CC3-BB55-4B781A5FB880}"/>
-    <hyperlink ref="G15" r:id="rId2" xr:uid="{A16AB8A1-67CA-4A8A-AEDB-1145814368C5}"/>
-    <hyperlink ref="G24" r:id="rId3" xr:uid="{4968C7B2-30C1-44A8-8572-F6C3CDABDA01}"/>
-    <hyperlink ref="G25" r:id="rId4" xr:uid="{D25871AB-2234-4A5A-858C-458E831639B4}"/>
+    <hyperlink ref="G14" r:id="rId2" xr:uid="{A16AB8A1-67CA-4A8A-AEDB-1145814368C5}"/>
+    <hyperlink ref="G23" r:id="rId3" xr:uid="{4968C7B2-30C1-44A8-8572-F6C3CDABDA01}"/>
+    <hyperlink ref="G24" r:id="rId4" xr:uid="{D25871AB-2234-4A5A-858C-458E831639B4}"/>
     <hyperlink ref="G2" r:id="rId5" xr:uid="{F739FC5B-84FF-47EC-843A-5D5A989F2E0C}"/>
     <hyperlink ref="G3" r:id="rId6" xr:uid="{F7C0B96C-3CA3-4F19-AADA-FECD5616754F}"/>
   </hyperlinks>

</xml_diff>